<commit_message>
- Updated regional aggregation relationship
</commit_message>
<xml_diff>
--- a/Input/SetoresGrupo.xlsx
+++ b/Input/SetoresGrupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinicius/Documents/IPEA/Python/MIP_Interregional_Haddad/Input_Vinicius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE50407B-A801-9949-BEA4-C1781A29A0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B092ED-E6C5-1444-BC65-0691E540A0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14560" windowHeight="18000" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetorGrupo" sheetId="42" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="180">
   <si>
     <t>Outros produtos alimentares</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>Metalurgia de metais não-ferrosos e a fundição de metais</t>
+  </si>
+  <si>
+    <t>Administração, defesa, educação e saúde públicas e seguridade social</t>
   </si>
 </sst>
 </file>
@@ -2260,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4087307C-9B7B-C843-B2B1-390DCBE4F481}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2765,7 +2768,7 @@
         <v>64</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>64</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.15">
@@ -2773,7 +2776,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
@@ -2789,7 +2792,7 @@
         <v>4</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>